<commit_message>
Changes pushed on 12th Jan 2020.
</commit_message>
<xml_diff>
--- a/PWRegressionSuite/src/main/java/testdata/PWData.xlsx
+++ b/PWRegressionSuite/src/main/java/testdata/PWData.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rganpisetty\workspace\PWRegressionSuite\src\main\java\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rganpisetty\git\PW\PWRegressionSuite\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51F2066-2C23-4155-AF2A-543F3F481491}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C750162-8C69-41F6-BCC1-84A118F66609}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D4E2F267-5BB4-4FD4-8E7A-B16EA4FB5ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="1" r:id="rId1"/>
+    <sheet name="Leases" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,31 +32,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Unit Name</t>
   </si>
   <si>
-    <t>Suit101</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Luxury Suite with all amenities</t>
   </si>
   <si>
-    <t>dummy</t>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Yadav</t>
+  </si>
+  <si>
+    <t>Kuldeep</t>
+  </si>
+  <si>
+    <t>kuldeep.yadav@nomail.com</t>
+  </si>
+  <si>
+    <t>Suit260</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,14 +108,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -404,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18F78B7-B1AF-49D2-A0CC-D635A85EEFDF}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,23 +448,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E02102-F50B-4EB2-B13D-019DBCC09E40}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="23.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{E89F790E-7FAC-4722-AD88-0515420E7514}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding all the new files
</commit_message>
<xml_diff>
--- a/PWRegressionSuite/src/main/java/testdata/PWData.xlsx
+++ b/PWRegressionSuite/src/main/java/testdata/PWData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rganpisetty\git\PW\PWRegressionSuite\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C750162-8C69-41F6-BCC1-84A118F66609}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189D26D5-13BD-463E-A729-5E91D3AFEF22}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D4E2F267-5BB4-4FD4-8E7A-B16EA4FB5ED9}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{D4E2F267-5BB4-4FD4-8E7A-B16EA4FB5ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="1" r:id="rId1"/>
@@ -52,16 +52,16 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Yadav</t>
-  </si>
-  <si>
-    <t>Kuldeep</t>
-  </si>
-  <si>
-    <t>kuldeep.yadav@nomail.com</t>
-  </si>
-  <si>
     <t>Suit260</t>
+  </si>
+  <si>
+    <t>Kohli</t>
+  </si>
+  <si>
+    <t>Virat</t>
+  </si>
+  <si>
+    <t>virat.kohli@nomail.com</t>
   </si>
 </sst>
 </file>
@@ -433,17 +433,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18F78B7-B1AF-49D2-A0CC-D635A85EEFDF}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" customWidth="1"/>
-    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,9 +451,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -468,18 +468,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E02102-F50B-4EB2-B13D-019DBCC09E40}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="23.7265625" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -490,20 +490,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{E89F790E-7FAC-4722-AD88-0515420E7514}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{733C911C-6AFE-428D-9E2A-0C7039A671F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pushed test cases ApplySecDepToCharges, new lease from Ledger and summary pages, rent bump and print ledger.
</commit_message>
<xml_diff>
--- a/PWRegressionSuite/src/main/java/testdata/PWData.xlsx
+++ b/PWRegressionSuite/src/main/java/testdata/PWData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rganpisetty\git\PW\PWRegressionSuite\src\main\java\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rganpisetty\workspace\PWRegressionSuite\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189D26D5-13BD-463E-A729-5E91D3AFEF22}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F58B75-B6A8-4AFA-8485-1E34BF73762F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{D4E2F267-5BB4-4FD4-8E7A-B16EA4FB5ED9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D4E2F267-5BB4-4FD4-8E7A-B16EA4FB5ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="1" r:id="rId1"/>
@@ -55,13 +55,13 @@
     <t>Suit260</t>
   </si>
   <si>
-    <t>Kohli</t>
-  </si>
-  <si>
-    <t>Virat</t>
-  </si>
-  <si>
-    <t>virat.kohli@nomail.com</t>
+    <t>Abdul</t>
+  </si>
+  <si>
+    <t>Kalam</t>
+  </si>
+  <si>
+    <t>abdul.kalam@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -437,13 +437,13 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -469,17 +469,17 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -490,12 +490,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added test cases for EmailTenantsTest and Views
</commit_message>
<xml_diff>
--- a/PWRegressionSuite/src/main/java/testdata/PWData.xlsx
+++ b/PWRegressionSuite/src/main/java/testdata/PWData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rganpisetty\workspace\PWRegressionSuite\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5CA67A-F1E0-428A-ACC5-38263E5808B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5E2D6A-011A-4E30-A7ED-CA11220478EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D4E2F267-5BB4-4FD4-8E7A-B16EA4FB5ED9}"/>
   </bookViews>
@@ -55,13 +55,13 @@
     <t>Suit260</t>
   </si>
   <si>
-    <t>Ratan</t>
-  </si>
-  <si>
-    <t>Tata</t>
-  </si>
-  <si>
-    <t>ratan.tata@gmail.com</t>
+    <t>Chandra</t>
+  </si>
+  <si>
+    <t>Siddarth</t>
+  </si>
+  <si>
+    <t>chandra.siddarth@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>